<commit_message>
Update Distribution of Aberrant T Cells
</commit_message>
<xml_diff>
--- a/1_Data Cleaning/distribution of immune receptors.xlsx
+++ b/1_Data Cleaning/distribution of immune receptors.xlsx
@@ -80,7 +80,7 @@
     <t xml:space="preserve">all_a_b_g_d_NA</t>
   </si>
   <si>
-    <t xml:space="preserve">Act. Tγδ</t>
+    <t xml:space="preserve">Act. Tgd</t>
   </si>
   <si>
     <t xml:space="preserve">Act. plasma IGHA+</t>
@@ -143,7 +143,7 @@
     <t xml:space="preserve">Mem B cells</t>
   </si>
   <si>
-    <t xml:space="preserve">NK/Tγδ</t>
+    <t xml:space="preserve">NK/Tgd</t>
   </si>
   <si>
     <t xml:space="preserve">Plasma IGHG+</t>
@@ -158,6 +158,12 @@
     <t xml:space="preserve">Tfh</t>
   </si>
   <si>
+    <t xml:space="preserve">Tgd CD8+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tgd INSIG1+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Th17</t>
   </si>
   <si>
@@ -165,12 +171,6 @@
   </si>
   <si>
     <t xml:space="preserve">Trm IEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tγδ CD8+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tγδ INSIG1+</t>
   </si>
   <si>
     <t xml:space="preserve">nIEL</t>
@@ -2349,67 +2349,67 @@
         <v>48</v>
       </c>
       <c r="B28" t="n">
-        <v>15640</v>
+        <v>12265</v>
       </c>
       <c r="C28" t="n">
-        <v>5151</v>
+        <v>2910</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28" t="n">
-        <v>32</v>
+        <v>684</v>
       </c>
       <c r="F28" t="n">
-        <v>92</v>
+        <v>43</v>
       </c>
       <c r="G28" t="n">
-        <v>1481</v>
+        <v>644</v>
       </c>
       <c r="H28" t="n">
-        <v>3487</v>
+        <v>1287</v>
       </c>
       <c r="I28" t="n">
-        <v>337</v>
+        <v>788</v>
       </c>
       <c r="J28" t="n">
-        <v>29</v>
+        <v>172</v>
       </c>
       <c r="K28" t="n">
-        <v>4013</v>
+        <v>1210</v>
       </c>
       <c r="L28" t="n">
-        <v>214</v>
+        <v>499</v>
       </c>
       <c r="M28" t="n">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="N28" t="n">
-        <v>578</v>
+        <v>922</v>
       </c>
       <c r="O28" t="n">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="P28" t="n">
-        <v>12</v>
+        <v>365</v>
       </c>
       <c r="Q28" t="n">
-        <v>1063</v>
+        <v>1511</v>
       </c>
       <c r="R28" t="n">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="S28" t="n">
-        <v>5</v>
+        <v>69</v>
       </c>
       <c r="T28" t="n">
-        <v>15</v>
+        <v>192</v>
       </c>
       <c r="U28" t="n">
-        <v>50</v>
+        <v>191</v>
       </c>
       <c r="V28" t="n">
-        <v>4194</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="29">
@@ -2417,67 +2417,67 @@
         <v>49</v>
       </c>
       <c r="B29" t="n">
-        <v>4891</v>
+        <v>1804</v>
       </c>
       <c r="C29" t="n">
-        <v>2211</v>
+        <v>333</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>3</v>
+        <v>711</v>
       </c>
       <c r="F29" t="n">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="G29" t="n">
-        <v>388</v>
+        <v>26</v>
       </c>
       <c r="H29" t="n">
-        <v>1136</v>
+        <v>102</v>
       </c>
       <c r="I29" t="n">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="J29" t="n">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="K29" t="n">
-        <v>2043</v>
+        <v>120</v>
       </c>
       <c r="L29" t="n">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="M29" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N29" t="n">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="O29" t="n">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="P29" t="n">
-        <v>1</v>
+        <v>365</v>
       </c>
       <c r="Q29" t="n">
-        <v>121</v>
+        <v>233</v>
       </c>
       <c r="R29" t="n">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="S29" t="n">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="T29" t="n">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="U29" t="n">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="V29" t="n">
-        <v>1033</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30">
@@ -2485,67 +2485,67 @@
         <v>50</v>
       </c>
       <c r="B30" t="n">
-        <v>10961</v>
+        <v>15640</v>
       </c>
       <c r="C30" t="n">
-        <v>2853</v>
+        <v>5151</v>
       </c>
       <c r="D30" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>1259</v>
+        <v>32</v>
       </c>
       <c r="F30" t="n">
-        <v>834</v>
+        <v>92</v>
       </c>
       <c r="G30" t="n">
-        <v>500</v>
+        <v>1481</v>
       </c>
       <c r="H30" t="n">
-        <v>993</v>
+        <v>3487</v>
       </c>
       <c r="I30" t="n">
-        <v>799</v>
+        <v>337</v>
       </c>
       <c r="J30" t="n">
-        <v>353</v>
+        <v>29</v>
       </c>
       <c r="K30" t="n">
-        <v>1060</v>
+        <v>4013</v>
       </c>
       <c r="L30" t="n">
-        <v>482</v>
+        <v>214</v>
       </c>
       <c r="M30" t="n">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="N30" t="n">
-        <v>883</v>
+        <v>578</v>
       </c>
       <c r="O30" t="n">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="P30" t="n">
-        <v>828</v>
+        <v>12</v>
       </c>
       <c r="Q30" t="n">
-        <v>1749</v>
+        <v>1063</v>
       </c>
       <c r="R30" t="n">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="S30" t="n">
-        <v>109</v>
+        <v>5</v>
       </c>
       <c r="T30" t="n">
-        <v>300</v>
+        <v>15</v>
       </c>
       <c r="U30" t="n">
-        <v>222</v>
+        <v>50</v>
       </c>
       <c r="V30" t="n">
-        <v>2518</v>
+        <v>4194</v>
       </c>
     </row>
     <row r="31">
@@ -2553,67 +2553,67 @@
         <v>51</v>
       </c>
       <c r="B31" t="n">
-        <v>12265</v>
+        <v>4891</v>
       </c>
       <c r="C31" t="n">
-        <v>2910</v>
+        <v>2211</v>
       </c>
       <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
         <v>3</v>
       </c>
-      <c r="E31" t="n">
-        <v>684</v>
-      </c>
       <c r="F31" t="n">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="G31" t="n">
-        <v>644</v>
+        <v>388</v>
       </c>
       <c r="H31" t="n">
-        <v>1287</v>
+        <v>1136</v>
       </c>
       <c r="I31" t="n">
-        <v>788</v>
+        <v>21</v>
       </c>
       <c r="J31" t="n">
-        <v>172</v>
+        <v>8</v>
       </c>
       <c r="K31" t="n">
-        <v>1210</v>
+        <v>2043</v>
       </c>
       <c r="L31" t="n">
-        <v>499</v>
+        <v>12</v>
       </c>
       <c r="M31" t="n">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="N31" t="n">
-        <v>922</v>
+        <v>45</v>
       </c>
       <c r="O31" t="n">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="P31" t="n">
-        <v>365</v>
+        <v>1</v>
       </c>
       <c r="Q31" t="n">
-        <v>1511</v>
+        <v>121</v>
       </c>
       <c r="R31" t="n">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="S31" t="n">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="T31" t="n">
-        <v>192</v>
+        <v>2</v>
       </c>
       <c r="U31" t="n">
-        <v>191</v>
+        <v>18</v>
       </c>
       <c r="V31" t="n">
-        <v>4226</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="32">
@@ -2621,67 +2621,67 @@
         <v>52</v>
       </c>
       <c r="B32" t="n">
-        <v>1804</v>
+        <v>10961</v>
       </c>
       <c r="C32" t="n">
-        <v>333</v>
+        <v>2853</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E32" t="n">
-        <v>711</v>
+        <v>1259</v>
       </c>
       <c r="F32" t="n">
-        <v>104</v>
+        <v>834</v>
       </c>
       <c r="G32" t="n">
-        <v>26</v>
+        <v>500</v>
       </c>
       <c r="H32" t="n">
-        <v>102</v>
+        <v>993</v>
       </c>
       <c r="I32" t="n">
-        <v>95</v>
+        <v>799</v>
       </c>
       <c r="J32" t="n">
-        <v>82</v>
+        <v>353</v>
       </c>
       <c r="K32" t="n">
-        <v>120</v>
+        <v>1060</v>
       </c>
       <c r="L32" t="n">
-        <v>54</v>
+        <v>482</v>
       </c>
       <c r="M32" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="N32" t="n">
-        <v>137</v>
+        <v>883</v>
       </c>
       <c r="O32" t="n">
-        <v>37</v>
+        <v>101</v>
       </c>
       <c r="P32" t="n">
-        <v>365</v>
+        <v>828</v>
       </c>
       <c r="Q32" t="n">
-        <v>233</v>
+        <v>1749</v>
       </c>
       <c r="R32" t="n">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="S32" t="n">
-        <v>42</v>
+        <v>109</v>
       </c>
       <c r="T32" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="U32" t="n">
-        <v>115</v>
+        <v>222</v>
       </c>
       <c r="V32" t="n">
-        <v>179</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="33">

</xml_diff>